<commit_message>
Auto stash before rebase of "refs/heads/develop"
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biti9\Documents\UiPath\ReFramework_UiDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC71179-40F0-48D7-A77E-1041F049063C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE68E17-CBA6-462E-A666-CAF8B7BF8B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3831" yWindow="1337" windowWidth="16458" windowHeight="9549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -116,10 +116,16 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>tableTransaction</t>
+    <t>UiDemoPath</t>
   </si>
   <si>
-    <t>UiDemoPath</t>
+    <t>UiDemoCredential</t>
+  </si>
+  <si>
+    <t>credencial-UiDemo</t>
+  </si>
+  <si>
+    <t>data_queue_transaction</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1"/>
@@ -542,13 +548,20 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
         <v>26</v>
@@ -2725,10 +2738,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>